<commit_message>
adding multiple columns primary key support
</commit_message>
<xml_diff>
--- a/testDBs/UWV_case_1/csv_schema.xlsx
+++ b/testDBs/UWV_case_1/csv_schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\event-log-extraction-assistant\testDBs\UWV_case_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D030203-D59E-496E-9A84-DD780632EE6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98212ED8-9721-4FF8-BD2D-BC881D54EDC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12900" yWindow="5565" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9150" yWindow="4155" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="24">
   <si>
     <t>table_name</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>ActivityID_507</t>
+  </si>
+  <si>
+    <t>data_type</t>
+  </si>
+  <si>
+    <t>ActivityID</t>
+  </si>
+  <si>
+    <t>Attribute_101</t>
   </si>
 </sst>
 </file>
@@ -414,22 +423,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -437,27 +447,30 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -467,43 +480,46 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -512,20 +528,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
@@ -534,78 +550,78 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
         <v>17</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>19</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
@@ -616,9 +632,31 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
         <v>20</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C19" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>